<commit_message>
Adicionado horário de execução do script
</commit_message>
<xml_diff>
--- a/url1.xlsx
+++ b/url1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="80">
   <si>
     <t>title</t>
   </si>
@@ -34,214 +34,226 @@
     <t>superhost</t>
   </si>
   <si>
+    <t>execution_time</t>
+  </si>
+  <si>
     <t>Casa em Araruama</t>
   </si>
   <si>
+    <t>Apartamento em Araruama</t>
+  </si>
+  <si>
+    <t>Casa em Fazendinha</t>
+  </si>
+  <si>
     <t>Casa em Parque Hotel</t>
   </si>
   <si>
-    <t>Apartamento em Araruama</t>
-  </si>
-  <si>
-    <t>Casa em Fazendinha</t>
+    <t>Chalé em Coqueiral</t>
   </si>
   <si>
     <t>Casa de campo em Praia Seca</t>
   </si>
   <si>
-    <t>Chalé em Coqueiral</t>
+    <t>Quarto privativo em Araruama</t>
   </si>
   <si>
     <t>Casa de campo em Outeiro</t>
   </si>
   <si>
-    <t>Quarto privativo em Araruama</t>
-  </si>
-  <si>
     <t>Região dos lagos - Araruama - Saquarema - Arraial</t>
   </si>
   <si>
+    <t>Casa em Araruama 1</t>
+  </si>
+  <si>
+    <t>Casa tranquila, bem localizada Ar opcional Tv wifi</t>
+  </si>
+  <si>
+    <t>Pedacinho do Céu</t>
+  </si>
+  <si>
+    <t>Apartamento em frente a lagoa de Araruama</t>
+  </si>
+  <si>
+    <t>Casa em Araruama 2</t>
+  </si>
+  <si>
     <t>Aconchegante Casa - Quintal &amp; Garagem</t>
   </si>
   <si>
-    <t>Casa em Araruama 1</t>
-  </si>
-  <si>
-    <t>Pedacinho do Céu</t>
+    <t>Chalé Recantinho da Lagoa, Araruama,Rj</t>
+  </si>
+  <si>
+    <t>Meu aconchego</t>
+  </si>
+  <si>
+    <t>Casa Maravilhosa com Lagoa privativa</t>
+  </si>
+  <si>
+    <t>loft &lt;SPA&lt; onde você descansa relaxa e se renova</t>
+  </si>
+  <si>
+    <t>Apto na Região dos lagos. Aconchegante e central.</t>
+  </si>
+  <si>
+    <t>VEM! Casa Rodrigues - Praia Seca, Araruama</t>
+  </si>
+  <si>
+    <t>Loft agradável em Araruama.</t>
   </si>
   <si>
     <t>Recanto para curtir e relaxar em Araruama</t>
   </si>
   <si>
-    <t>Apartamento em frente a lagoa de Araruama</t>
-  </si>
-  <si>
-    <t>Casa tranquila, bem localizada Ar opcional Tv wifi</t>
-  </si>
-  <si>
-    <t>loft &lt;SPA&lt; onde você descansa relaxa e se renova</t>
-  </si>
-  <si>
-    <t>Meu aconchego</t>
-  </si>
-  <si>
-    <t>Casa em Araruama 2</t>
-  </si>
-  <si>
-    <t>Casa Maravilhosa com Lagoa privativa</t>
-  </si>
-  <si>
-    <t>Chalé Recantinho da Lagoa, Araruama,Rj</t>
-  </si>
-  <si>
     <t>Casa com piscina no Condomínio Sonho de Vida</t>
   </si>
   <si>
-    <t>Apto na Região dos lagos. Aconchegante e central.</t>
-  </si>
-  <si>
     <t>Suíte aconchegante no centro de Praia Seca.</t>
   </si>
   <si>
-    <t>Curta o melhor de Araruama e Região dos Lagos</t>
-  </si>
-  <si>
-    <t>VEM! Casa Rodrigues - Praia Seca, Araruama</t>
-  </si>
-  <si>
     <t>Aluguel por temporada com piscina privativa</t>
   </si>
   <si>
     <t>2 camas de casal</t>
   </si>
   <si>
+    <t>4 camas</t>
+  </si>
+  <si>
+    <t>2 camas</t>
+  </si>
+  <si>
+    <t>1 cama de casal</t>
+  </si>
+  <si>
     <t>1 cama queen</t>
   </si>
   <si>
-    <t>4 camas</t>
-  </si>
-  <si>
-    <t>1 cama de casal</t>
-  </si>
-  <si>
     <t>3 camas</t>
   </si>
   <si>
-    <t>2 camas</t>
-  </si>
-  <si>
     <t>9 camas</t>
   </si>
   <si>
     <t>3 camas de casal</t>
   </si>
   <si>
-    <t>R$110 por noite</t>
+    <t>1 cama</t>
+  </si>
+  <si>
+    <t>R$114 por noite</t>
+  </si>
+  <si>
+    <t>R$106 por noite</t>
+  </si>
+  <si>
+    <t>R$118 por noite</t>
+  </si>
+  <si>
+    <t>R$85 por noite, originalmente R$93</t>
+  </si>
+  <si>
+    <t>R$173 por noite, originalmente R$211</t>
+  </si>
+  <si>
+    <t>R$98 por noite, originalmente R$109</t>
   </si>
   <si>
     <t>R$137 por noite</t>
   </si>
   <si>
-    <t>R$106 por noite</t>
-  </si>
-  <si>
-    <t>R$96 por noite</t>
+    <t>R$91 por noite</t>
+  </si>
+  <si>
+    <t>R$189 por noite, originalmente R$235</t>
+  </si>
+  <si>
+    <t>R$116 por noite</t>
+  </si>
+  <si>
+    <t>R$189 por noite, originalmente R$301</t>
+  </si>
+  <si>
+    <t>R$140 por noite</t>
+  </si>
+  <si>
+    <t>R$110 por noite, originalmente R$135</t>
+  </si>
+  <si>
+    <t>R$131 por noite</t>
   </si>
   <si>
     <t>R$210 por noite</t>
   </si>
   <si>
-    <t>R$173 por noite, originalmente R$211</t>
-  </si>
-  <si>
-    <t>R$118 por noite</t>
-  </si>
-  <si>
-    <t>R$189 por noite, originalmente R$302</t>
-  </si>
-  <si>
-    <t>R$187 por noite, originalmente R$235</t>
-  </si>
-  <si>
-    <t>R$117 por noite</t>
-  </si>
-  <si>
-    <t>R$91 por noite</t>
-  </si>
-  <si>
     <t>R$290 por noite, originalmente R$352</t>
   </si>
   <si>
-    <t>R$140 por noite</t>
-  </si>
-  <si>
     <t>R$136 por noite, originalmente R$166</t>
   </si>
   <si>
-    <t>R$133 por noite</t>
-  </si>
-  <si>
-    <t>R$116 por noite, originalmente R$137</t>
-  </si>
-  <si>
     <t>R$315 por noite</t>
   </si>
   <si>
     <t>4,79 (282)</t>
   </si>
   <si>
+    <t>4,97 (159)</t>
+  </si>
+  <si>
+    <t>4,9 (21)</t>
+  </si>
+  <si>
+    <t>4,92 (12)</t>
+  </si>
+  <si>
+    <t>4,85 (26)</t>
+  </si>
+  <si>
+    <t>5,0 (27)</t>
+  </si>
+  <si>
     <t>4,89 (46)</t>
   </si>
   <si>
-    <t>4,97 (158)</t>
-  </si>
-  <si>
-    <t>4,92 (12)</t>
+    <t>4,84 (75)</t>
+  </si>
+  <si>
+    <t>4,9 (10)</t>
+  </si>
+  <si>
+    <t>4,77 (22)</t>
+  </si>
+  <si>
+    <t>5,0 (9)</t>
+  </si>
+  <si>
+    <t>4,71 (7)</t>
+  </si>
+  <si>
+    <t>4,92 (173)</t>
+  </si>
+  <si>
+    <t>Novo</t>
   </si>
   <si>
     <t>5,0 (29)</t>
   </si>
   <si>
-    <t>4,85 (26)</t>
-  </si>
-  <si>
-    <t>4,9 (21)</t>
-  </si>
-  <si>
-    <t>5,0 (9)</t>
-  </si>
-  <si>
-    <t>4,89 (9)</t>
-  </si>
-  <si>
-    <t>5,0 (26)</t>
-  </si>
-  <si>
-    <t>4,75 (20)</t>
-  </si>
-  <si>
-    <t>4,84 (75)</t>
-  </si>
-  <si>
     <t>5,0 (21)</t>
   </si>
   <si>
-    <t>4,71 (7)</t>
-  </si>
-  <si>
     <t>5,0 (11)</t>
   </si>
   <si>
-    <t>4,89 (28)</t>
-  </si>
-  <si>
-    <t>4,92 (173)</t>
-  </si>
-  <si>
-    <t>4,97 (66)</t>
+    <t>4,97 (67)</t>
   </si>
   <si>
     <t>Superhost</t>
+  </si>
+  <si>
+    <t>24/04/2023 21:45:58</t>
   </si>
 </sst>
 </file>
@@ -599,13 +611,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -624,347 +636,401 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>60</v>
+      </c>
+      <c r="G2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="F3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>78</v>
+      </c>
+      <c r="G3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F5" t="s">
+        <v>78</v>
+      </c>
+      <c r="G5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" t="s">
+        <v>64</v>
+      </c>
+      <c r="G6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
         <v>34</v>
       </c>
-      <c r="D4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E4" t="s">
-        <v>59</v>
-      </c>
-      <c r="F4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E5" t="s">
-        <v>60</v>
-      </c>
-      <c r="F5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E6" t="s">
-        <v>61</v>
-      </c>
-      <c r="F6" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" t="s">
-        <v>37</v>
-      </c>
       <c r="D7" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+        <v>65</v>
+      </c>
+      <c r="F7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
         <v>37</v>
       </c>
       <c r="D8" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E8" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="F8" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>78</v>
+      </c>
+      <c r="G8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D9" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E9" t="s">
-        <v>64</v>
-      </c>
-      <c r="F9" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <v>67</v>
+      </c>
+      <c r="G9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" t="s">
+        <v>68</v>
+      </c>
+      <c r="G10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" t="s">
+        <v>69</v>
+      </c>
+      <c r="G11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" t="s">
+        <v>70</v>
+      </c>
+      <c r="F12" t="s">
+        <v>78</v>
+      </c>
+      <c r="G12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" t="s">
+        <v>71</v>
+      </c>
+      <c r="G13" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" t="s">
+        <v>54</v>
+      </c>
+      <c r="E14" t="s">
+        <v>72</v>
+      </c>
+      <c r="F14" t="s">
+        <v>78</v>
+      </c>
+      <c r="G14" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" t="s">
+        <v>73</v>
+      </c>
+      <c r="G15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" t="s">
         <v>38</v>
       </c>
-      <c r="D10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E10" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E11" t="s">
-        <v>66</v>
-      </c>
-      <c r="F11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" t="s">
-        <v>39</v>
-      </c>
-      <c r="D12" t="s">
-        <v>49</v>
-      </c>
-      <c r="E12" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" t="s">
-        <v>50</v>
-      </c>
-      <c r="E13" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" t="s">
-        <v>51</v>
-      </c>
-      <c r="E14" t="s">
-        <v>69</v>
-      </c>
-      <c r="F14" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15" t="s">
-        <v>52</v>
-      </c>
-      <c r="E15" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" t="s">
-        <v>35</v>
-      </c>
       <c r="D16" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="E16" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="F16" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+        <v>78</v>
+      </c>
+      <c r="G16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C17" t="s">
         <v>34</v>
       </c>
       <c r="D17" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E17" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="F17" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+        <v>78</v>
+      </c>
+      <c r="G17" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
         <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C18" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D18" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E18" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="F18" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+        <v>78</v>
+      </c>
+      <c r="G18" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B19" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C19" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D19" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="E19" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F19" t="s">
-        <v>75</v>
+        <v>78</v>
+      </c>
+      <c r="G19" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>